<commit_message>
Update Data Structures & Algorithms.xlsx
</commit_message>
<xml_diff>
--- a/Data Structures & Algorithms.xlsx
+++ b/Data Structures & Algorithms.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="266">
   <si>
     <t>Video Solution</t>
   </si>
@@ -201,6 +201,66 @@
   </si>
   <si>
     <t>Iterate through the array and maintain a running sum. If the sum becomes negative, reset it to 0, effectively starting a new subarray. At each step, update a global maximum (maxSum) to track the largest sum encountered.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/excAOvwF_Wk</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
+  </si>
+  <si>
+    <t>Find the maximum profit by tracking the minimum price so far and calculating the maximum difference (profit) between the current price and the minimum price.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/h4aBagy4Uok</t>
+  </si>
+  <si>
+    <t>2149. Rearrange Array Elements by Sign</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rearrange-array-elements-by-sign/description/</t>
+  </si>
+  <si>
+    <t>Just take an extra array and iterate the given array and keep inserting the positive elements at even places and negative elements at odd places.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/JDOXKqF60RQ</t>
+  </si>
+  <si>
+    <t>31. Next Permutation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/total-characters-in-string-after-transformations-i/description/?envType=daily-question&amp;envId=2025-05-13</t>
+  </si>
+  <si>
+    <t>Find the first decreasing element from the right, swap it with the next larger element to its right, then reverse the subarray after its original position to get the next lexicographical permutation.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/oO5uLE7EUlM</t>
+  </si>
+  <si>
+    <t>128. Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-consecutive-sequence/description/</t>
+  </si>
+  <si>
+    <t>Store the numbers in a set, for each number, if it's the start of a sequence (no num-1 in set), count the length of consecutive numbers starting from it, and track the maximum found.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/N0MgLvceX7M</t>
+  </si>
+  <si>
+    <t>73. Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/set-matrix-zeroes/description/</t>
+  </si>
+  <si>
+    <t>Use the first row and first column as markers to record which rows and columns should be zeroed, and a separate variable for the first column. In the first pass, mark the corresponding row and column if a zero is found. In the second pass, set matrix cells to zero based on these markers, then update the first row and column if needed.</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=eD3tmO66aBA&amp;list=PLgUwDviBIf0oF6QL8m22w1hIDC1vJ_BHz&amp;index=86&amp;pp=iAQB</t>
@@ -879,6 +939,439 @@
         <color theme="1"/>
       </rPr>
       <t>Use a prev array to store the maximum points up to the previous day, and update it iteratively for each day using a temporary array temp. The final result is stored in prev[3].</t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/sdE0A2Oxofw?si=VELB0uSV76Z_F9R5</t>
+  </si>
+  <si>
+    <t>62. Unique Paths</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/description/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Starting from end we can either go to left or up, just travel left or up using recursion and if we reach end i.e (0,0) then return 1 and store it in dp array. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D table to store paths to reach the current index. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation + Space Optimization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a prev array to store to the curr row after it is processed and then make it the prev row and initialize the curr row as 0 or -1.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/TmhpgXScLyY</t>
+  </si>
+  <si>
+    <t>63. Unique Paths II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths-ii/description/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Starting from end we can either go to left or up, just travel left or up using recursion and if we reach end i.e (0,0) then return 1 and store it in dp array and return 0 and store it in dp array if obstacle[i][j] = 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D table to store paths to reach the current index. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation + Space Optimization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a prev array to store to the curr row after it is processed and then make it the prev row and initialize the curr row as 0 or -1.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/_rgTlyky1uQ?si=qXOSFWT36e9hFlAR</t>
+  </si>
+  <si>
+    <t>64. Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-path-sum/description/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Starting from end we can either go to left or up, just travel left or up using recursion and if we reach end i.e (0,0) then return the value at (0,0) and store it in dp array and return store min(up, left) in dp array. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D table to store min path length to reach the current index. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation + Space Optimization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a prev array to store to the curr row after it is processed and then make it the prev row and initialize the curr row as 0 or -1.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/SrP-PiLSYC0</t>
+  </si>
+  <si>
+    <t>120. Triangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/triangle/description/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Start from the top of the triangle (0,0). For each cell, calculate the minimum sum path recursively by moving either down or diagonally down-right, storing results in a `dp` array. Base case: last row of the triangle. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a `2D dp` array. Initialize the last row of `dp` as the last row of the triangle. For each cell in the triangle, move upwards, calculating the minimum path sum to that cell using values from the row below. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation + Space Optimization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Replace the `2D dp` table with two `1D arrays`: `prev` (current row) and `curr` (next row). After processing a row, make `curr` the new `prev`. Start with `prev` initialized to the last row of the triangle.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/N_aJ5qQbYA0?si=-FkikJ1RQQ68wcQI</t>
+  </si>
+  <si>
+    <t>931. Minimum Falling Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-falling-path-sum/description/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Start from the bottom row, recursively compute the minimum falling path sum by moving to `up`, `up-left`, and `up-right` from the current position. Use a `dp` table to store results of subproblems. Base case: reaching the first row. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a `2D dp` array to compute the minimum falling path sum from the top to the bottom. Initialize the first row of `dp` as the first row of the matrix. For each cell, calculate the minimum sum to reach it from the row above. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Tabulation + Space Optimization: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Replace the `2D dp` array with two `1D arrays`: `prev` (previous row) and `curr` (current row). For each row, compute the minimum path sum using `prev` and update `curr`. After processing a row, make `curr` the new `prev`.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/QGfn7JeXK54?si=Fb-27MrTYcXRotRn</t>
+  </si>
+  <si>
+    <t>Chocolates Pickup</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/chocolates-pickup/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=chocolates-pickup</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Memoization: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Use a 3D `dp` array to store the maximum chocolates collected by two robots starting from `(0, 0)` and `(0, m-1)` and moving downward. For each cell `(i, j1, j2)`, recursively calculate the maximum chocolates the two robots can collect by trying all possible moves (`-1`, `0`, `+1`) for both robots. Base case: If `j1` or `j2` goes out of bounds, return `-1e8`. If at the last row, return the sum of chocolates at `j1` and `j2` (considering overlap). Store the result in `dp[i][j1][j2]` to avoid redundant calculations. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Tabulation: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Use a 3D `dp` array where `dp[i][j1][j2]` represents the maximum chocolates collected by the two robots starting at row `i`, columns `j1` and `j2`. Initialize the last row in `dp` with the chocolates collected at the respective positions. For each row from `n-2` to `0`, calculate the maximum chocolates collected by considering all valid moves (`-1`, `0`, `+1`) for both robots. Use nested loops for `j1`, `j2`, and the moves of both robots to calculate `dp[i][j1][j2]`. Return `dp[0][0][m-1]`, which represents the maximum chocolates collected by the robots starting at the top-left (`0, 0`) and top-right (`0, m-1`).  </t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/fWX9xDmIzRI</t>
+  </si>
+  <si>
+    <t>Subset Sum Problem</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/subset-sum-problem-1611555638/1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D `dp` array where `dp[i][target]` stores whether it's possible to form `target` using the first `i` elements. Base cases: If `target == 0`, return `true` (an empty subset sums to `0`). If `i == 0`, return whether `arr[0] == target`. For each index `i`, consider two choices: 1. Not take the current element (`helper(i-1, arr, target, dp)`). 2. Take** the current element if `arr[i] &lt;= target` (`helper(i-1, arr, target - arr[i], dp)`). Combine results using logical OR (`|`). Store the result in `dp[i][target]` to avoid redundant calculations. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D `dp` array where `dp[i][j]` is `true` if it's possible to form sum `j` using the first `i` elements. Initialize base cases: `dp[i][0] = true` for all `i` (sum `0` is always possible). If `arr[0] &lt;= target`, set `dp[0][arr[0]] = true`.  Iterate through the array and for each index `ind` and target sum `j`: 1. Not take: Use the result from the previous row (`dp[ind-1][j]`). 2.Take: Use `dp[ind-1][j - arr[ind]]` if `arr[ind] &lt;= j`. Final result is in `dp[n-1][target]`. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation + Space Optimization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 1D `prev` array to store results for the previous row. Initialize `prev[0] = true` (sum `0` is always possible). Update the `prev` array row by row using a temporary `curr` array. For each `ind` and sum `j`: 1. Not take: `prev[j]`. 2. Take: `prev[j - arr[ind]]` if `arr[ind] &lt;= j`. At the end of each iteration, copy `curr` to `prev`. The result is in `prev[target]`.  </t>
+    </r>
+  </si>
+  <si>
+    <t>https://youtu.be/7win3dcgo3k?si=dqTM8TEZfKqBD43t</t>
+  </si>
+  <si>
+    <t>416. Partition Equal Subset Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/partition-equal-subset-sum/description/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Memoization:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D `dp` array where `dp[i][target]` represents whether it's possible to form a subset with sum `target` using the first `i` elements. Base cases: If `target == 0`, return `true` (a subset with sum `0` is always possible). If `i == 0`, check if `nums[0] == target`. For each index `i`, consider two choices: 1. Not take** the current element (`helper(i - 1, target, nums, dp)`). 2. Take** the current element if `nums[i] &lt;= target` (`helper(i - 1, target - nums[i], nums, dp)`). Combine results using logical OR (`|`). Store the result in `dp[i][target]` to avoid redundant calculations. Initial Setup: Compute the total sum of the array. If it's odd, return `false` (not possible to partition). Call the helper function with `target = sum / 2` to check if a subset with that sum exists. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabulation:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Use a 2D `dp` array where `dp[i][j]` is `true` if it's possible to form a subset with sum `j` using the first `i` elements. Base cases: `dp[i][0] = true` for all `i` (sum `0` is always possible). If `nums[0] &lt;= target`, set `dp[0][nums[0]] = true`. Iterate through the array and for each index `ind` and target sum `j`: 1. Not take**: Use the result from the previous row (`dp[ind - 1][j]`). 2. Take: Use `dp[ind - 1][j - nums[ind]]` if `nums[ind] &lt;= j`. Final result: Check `dp[n-1][target]`. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Tabulation + Space Optimization: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Use a 1D `prev` array to store results for the previous row. Base cases: `prev[0] = true` (sum `0` is always possible). If `nums[0] &lt;= target`, set `prev[nums[0]] = true`. Update the `prev` array row by row using a temporary `curr` array. For each `ind` and sum `j`: 1. Not take: `prev[j]`. 2. Take: `prev[j - nums[ind]]` if `nums[ind] &lt;= j`.  At the end of each iteration, copy `curr` to `prev`. Final result: Check `prev[target]`.</t>
     </r>
   </si>
 </sst>
@@ -1511,34 +2004,89 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="A22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="12"/>
@@ -2120,461 +2668,461 @@
     </row>
     <row r="110">
       <c r="A110" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="9" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="9" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="9" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="9" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="9" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="3" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="3" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="3" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="9" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="3" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="3" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="3" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="3" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="3" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="3" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="137">
@@ -2629,82 +3177,82 @@
     <row r="144">
       <c r="A144" s="6"/>
       <c r="B144" s="4" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="6"/>
       <c r="B145" s="4" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="3" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="3" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="3" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
     </row>
     <row r="149">
@@ -2912,178 +3460,258 @@
     </row>
     <row r="178">
       <c r="A178" s="3" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="3" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="3" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="9" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="3" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B183" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B183" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="C183" s="7" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="9" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="12"/>
-      <c r="B185" s="13"/>
-      <c r="C185" s="12"/>
-      <c r="D185" s="12"/>
-      <c r="E185" s="12"/>
+      <c r="A185" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C185" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D185" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="186">
-      <c r="A186" s="12"/>
-      <c r="B186" s="13"/>
-      <c r="C186" s="12"/>
-      <c r="D186" s="12"/>
-      <c r="E186" s="12"/>
+      <c r="A186" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="187">
-      <c r="A187" s="12"/>
-      <c r="B187" s="13"/>
-      <c r="C187" s="12"/>
-      <c r="D187" s="12"/>
-      <c r="E187" s="12"/>
+      <c r="A187" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D187" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="188">
-      <c r="A188" s="12"/>
-      <c r="B188" s="13"/>
-      <c r="C188" s="12"/>
-      <c r="D188" s="12"/>
-      <c r="E188" s="12"/>
+      <c r="A188" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C188" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E188" s="6" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="189">
-      <c r="A189" s="12"/>
-      <c r="B189" s="13"/>
-      <c r="C189" s="12"/>
-      <c r="D189" s="12"/>
-      <c r="E189" s="12"/>
+      <c r="A189" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="190">
-      <c r="A190" s="12"/>
-      <c r="B190" s="13"/>
-      <c r="C190" s="12"/>
-      <c r="D190" s="12"/>
-      <c r="E190" s="12"/>
+      <c r="A190" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C190" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="191">
-      <c r="A191" s="12"/>
-      <c r="B191" s="13"/>
-      <c r="C191" s="12"/>
-      <c r="D191" s="12"/>
-      <c r="E191" s="12"/>
+      <c r="A191" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="192">
-      <c r="A192" s="12"/>
-      <c r="B192" s="13"/>
-      <c r="C192" s="12"/>
-      <c r="D192" s="12"/>
-      <c r="E192" s="12"/>
+      <c r="A192" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C192" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="12"/>
@@ -8726,83 +9354,109 @@
     <hyperlink r:id="rId30" ref="D16"/>
     <hyperlink r:id="rId31" ref="A17"/>
     <hyperlink r:id="rId32" ref="D17"/>
-    <hyperlink r:id="rId33" ref="A110"/>
-    <hyperlink r:id="rId34" ref="D110"/>
-    <hyperlink r:id="rId35" ref="A111"/>
-    <hyperlink r:id="rId36" ref="D111"/>
-    <hyperlink r:id="rId37" ref="A112"/>
-    <hyperlink r:id="rId38" ref="D112"/>
-    <hyperlink r:id="rId39" ref="A113"/>
-    <hyperlink r:id="rId40" ref="D113"/>
-    <hyperlink r:id="rId41" ref="A114"/>
-    <hyperlink r:id="rId42" ref="D114"/>
-    <hyperlink r:id="rId43" ref="A115"/>
-    <hyperlink r:id="rId44" ref="D115"/>
-    <hyperlink r:id="rId45" ref="A116"/>
-    <hyperlink r:id="rId46" ref="D116"/>
-    <hyperlink r:id="rId47" ref="A117"/>
-    <hyperlink r:id="rId48" ref="D117"/>
-    <hyperlink r:id="rId49" ref="A118"/>
-    <hyperlink r:id="rId50" ref="D118"/>
-    <hyperlink r:id="rId51" ref="A119"/>
-    <hyperlink r:id="rId52" ref="D119"/>
-    <hyperlink r:id="rId53" ref="A120"/>
-    <hyperlink r:id="rId54" ref="D120"/>
-    <hyperlink r:id="rId55" ref="A121"/>
-    <hyperlink r:id="rId56" ref="D121"/>
-    <hyperlink r:id="rId57" ref="A122"/>
-    <hyperlink r:id="rId58" ref="D122"/>
-    <hyperlink r:id="rId59" ref="A123"/>
-    <hyperlink r:id="rId60" ref="D123"/>
-    <hyperlink r:id="rId61" ref="A124"/>
-    <hyperlink r:id="rId62" ref="D124"/>
-    <hyperlink r:id="rId63" ref="A125"/>
-    <hyperlink r:id="rId64" ref="D125"/>
-    <hyperlink r:id="rId65" ref="A126"/>
-    <hyperlink r:id="rId66" ref="D126"/>
-    <hyperlink r:id="rId67" ref="A127"/>
-    <hyperlink r:id="rId68" ref="D127"/>
-    <hyperlink r:id="rId69" ref="A128"/>
-    <hyperlink r:id="rId70" ref="D128"/>
-    <hyperlink r:id="rId71" ref="A129"/>
-    <hyperlink r:id="rId72" ref="D129"/>
-    <hyperlink r:id="rId73" ref="A130"/>
-    <hyperlink r:id="rId74" ref="D130"/>
-    <hyperlink r:id="rId75" ref="A131"/>
-    <hyperlink r:id="rId76" ref="D131"/>
-    <hyperlink r:id="rId77" ref="A132"/>
-    <hyperlink r:id="rId78" ref="D132"/>
-    <hyperlink r:id="rId79" ref="A133"/>
-    <hyperlink r:id="rId80" ref="D133"/>
-    <hyperlink r:id="rId81" ref="A134"/>
-    <hyperlink r:id="rId82" ref="D134"/>
-    <hyperlink r:id="rId83" ref="A135"/>
-    <hyperlink r:id="rId84" ref="D135"/>
-    <hyperlink r:id="rId85" ref="A136"/>
-    <hyperlink r:id="rId86" ref="D136"/>
-    <hyperlink r:id="rId87" ref="D144"/>
-    <hyperlink r:id="rId88" ref="D145"/>
-    <hyperlink r:id="rId89" ref="A146"/>
-    <hyperlink r:id="rId90" ref="D146"/>
-    <hyperlink r:id="rId91" ref="A147"/>
-    <hyperlink r:id="rId92" ref="D147"/>
-    <hyperlink r:id="rId93" ref="A148"/>
-    <hyperlink r:id="rId94" ref="D148"/>
-    <hyperlink r:id="rId95" ref="A178"/>
-    <hyperlink r:id="rId96" ref="D178"/>
-    <hyperlink r:id="rId97" ref="A179"/>
-    <hyperlink r:id="rId98" ref="D179"/>
-    <hyperlink r:id="rId99" ref="A180"/>
-    <hyperlink r:id="rId100" ref="D180"/>
-    <hyperlink r:id="rId101" ref="A181"/>
-    <hyperlink r:id="rId102" ref="D181"/>
-    <hyperlink r:id="rId103" ref="A182"/>
-    <hyperlink r:id="rId104" ref="D182"/>
-    <hyperlink r:id="rId105" ref="A183"/>
-    <hyperlink r:id="rId106" ref="D183"/>
-    <hyperlink r:id="rId107" ref="A184"/>
-    <hyperlink r:id="rId108" ref="D184"/>
+    <hyperlink r:id="rId33" ref="A18"/>
+    <hyperlink r:id="rId34" ref="D18"/>
+    <hyperlink r:id="rId35" ref="A19"/>
+    <hyperlink r:id="rId36" ref="D19"/>
+    <hyperlink r:id="rId37" ref="A20"/>
+    <hyperlink r:id="rId38" ref="D20"/>
+    <hyperlink r:id="rId39" ref="A21"/>
+    <hyperlink r:id="rId40" ref="D21"/>
+    <hyperlink r:id="rId41" ref="A22"/>
+    <hyperlink r:id="rId42" ref="D22"/>
+    <hyperlink r:id="rId43" ref="A110"/>
+    <hyperlink r:id="rId44" ref="D110"/>
+    <hyperlink r:id="rId45" ref="A111"/>
+    <hyperlink r:id="rId46" ref="D111"/>
+    <hyperlink r:id="rId47" ref="A112"/>
+    <hyperlink r:id="rId48" ref="D112"/>
+    <hyperlink r:id="rId49" ref="A113"/>
+    <hyperlink r:id="rId50" ref="D113"/>
+    <hyperlink r:id="rId51" ref="A114"/>
+    <hyperlink r:id="rId52" ref="D114"/>
+    <hyperlink r:id="rId53" ref="A115"/>
+    <hyperlink r:id="rId54" ref="D115"/>
+    <hyperlink r:id="rId55" ref="A116"/>
+    <hyperlink r:id="rId56" ref="D116"/>
+    <hyperlink r:id="rId57" ref="A117"/>
+    <hyperlink r:id="rId58" ref="D117"/>
+    <hyperlink r:id="rId59" ref="A118"/>
+    <hyperlink r:id="rId60" ref="D118"/>
+    <hyperlink r:id="rId61" ref="A119"/>
+    <hyperlink r:id="rId62" ref="D119"/>
+    <hyperlink r:id="rId63" ref="A120"/>
+    <hyperlink r:id="rId64" ref="D120"/>
+    <hyperlink r:id="rId65" ref="A121"/>
+    <hyperlink r:id="rId66" ref="D121"/>
+    <hyperlink r:id="rId67" ref="A122"/>
+    <hyperlink r:id="rId68" ref="D122"/>
+    <hyperlink r:id="rId69" ref="A123"/>
+    <hyperlink r:id="rId70" ref="D123"/>
+    <hyperlink r:id="rId71" ref="A124"/>
+    <hyperlink r:id="rId72" ref="D124"/>
+    <hyperlink r:id="rId73" ref="A125"/>
+    <hyperlink r:id="rId74" ref="D125"/>
+    <hyperlink r:id="rId75" ref="A126"/>
+    <hyperlink r:id="rId76" ref="D126"/>
+    <hyperlink r:id="rId77" ref="A127"/>
+    <hyperlink r:id="rId78" ref="D127"/>
+    <hyperlink r:id="rId79" ref="A128"/>
+    <hyperlink r:id="rId80" ref="D128"/>
+    <hyperlink r:id="rId81" ref="A129"/>
+    <hyperlink r:id="rId82" ref="D129"/>
+    <hyperlink r:id="rId83" ref="A130"/>
+    <hyperlink r:id="rId84" ref="D130"/>
+    <hyperlink r:id="rId85" ref="A131"/>
+    <hyperlink r:id="rId86" ref="D131"/>
+    <hyperlink r:id="rId87" ref="A132"/>
+    <hyperlink r:id="rId88" ref="D132"/>
+    <hyperlink r:id="rId89" ref="A133"/>
+    <hyperlink r:id="rId90" ref="D133"/>
+    <hyperlink r:id="rId91" ref="A134"/>
+    <hyperlink r:id="rId92" ref="D134"/>
+    <hyperlink r:id="rId93" ref="A135"/>
+    <hyperlink r:id="rId94" ref="D135"/>
+    <hyperlink r:id="rId95" ref="A136"/>
+    <hyperlink r:id="rId96" ref="D136"/>
+    <hyperlink r:id="rId97" ref="D144"/>
+    <hyperlink r:id="rId98" ref="D145"/>
+    <hyperlink r:id="rId99" ref="A146"/>
+    <hyperlink r:id="rId100" ref="D146"/>
+    <hyperlink r:id="rId101" ref="A147"/>
+    <hyperlink r:id="rId102" ref="D147"/>
+    <hyperlink r:id="rId103" ref="A148"/>
+    <hyperlink r:id="rId104" ref="D148"/>
+    <hyperlink r:id="rId105" ref="A178"/>
+    <hyperlink r:id="rId106" ref="D178"/>
+    <hyperlink r:id="rId107" ref="A179"/>
+    <hyperlink r:id="rId108" ref="D179"/>
+    <hyperlink r:id="rId109" ref="A180"/>
+    <hyperlink r:id="rId110" ref="D180"/>
+    <hyperlink r:id="rId111" ref="A181"/>
+    <hyperlink r:id="rId112" ref="D181"/>
+    <hyperlink r:id="rId113" ref="A182"/>
+    <hyperlink r:id="rId114" ref="D182"/>
+    <hyperlink r:id="rId115" ref="A183"/>
+    <hyperlink r:id="rId116" ref="D183"/>
+    <hyperlink r:id="rId117" ref="A184"/>
+    <hyperlink r:id="rId118" ref="D184"/>
+    <hyperlink r:id="rId119" ref="A185"/>
+    <hyperlink r:id="rId120" ref="D185"/>
+    <hyperlink r:id="rId121" ref="A186"/>
+    <hyperlink r:id="rId122" ref="D186"/>
+    <hyperlink r:id="rId123" ref="A187"/>
+    <hyperlink r:id="rId124" ref="D187"/>
+    <hyperlink r:id="rId125" ref="A188"/>
+    <hyperlink r:id="rId126" ref="D188"/>
+    <hyperlink r:id="rId127" ref="A189"/>
+    <hyperlink r:id="rId128" ref="D189"/>
+    <hyperlink r:id="rId129" ref="A190"/>
+    <hyperlink r:id="rId130" ref="D190"/>
+    <hyperlink r:id="rId131" ref="A191"/>
+    <hyperlink r:id="rId132" ref="D191"/>
+    <hyperlink r:id="rId133" ref="A192"/>
+    <hyperlink r:id="rId134" ref="D192"/>
   </hyperlinks>
-  <drawing r:id="rId109"/>
+  <drawing r:id="rId135"/>
 </worksheet>
 </file>
</xml_diff>